<commit_message>
added a missing entry vehID = 439
</commit_message>
<xml_diff>
--- a/Data/VED_Static_Data_ICE&HEV.xlsx
+++ b/Data/VED_Static_Data_ICE&HEV.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\gsoh_github\VED-master\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\3. Publication\Publication - VED\Source_code_VED\Data_Public\Files_Shared_Github_Backup\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E92557A6-4E05-4AC9-A893-F0BADE1CD4DE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D71940AC-986F-4253-A631-11B78527675B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="7728" xr2:uid="{22203255-1950-4A2E-87C1-49DAC957F055}"/>
+    <workbookView xWindow="3594" yWindow="2661" windowWidth="15783" windowHeight="9032" xr2:uid="{22203255-1950-4A2E-87C1-49DAC957F055}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1800" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1805" uniqueCount="101">
   <si>
     <t>VehId</t>
   </si>
@@ -684,19 +684,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8D7BCA2-6EC1-4D1F-8A55-6EB58888BFCD}">
-  <dimension ref="A1:G357"/>
+  <dimension ref="A1:G358"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A319" workbookViewId="0">
-      <selection activeCell="I356" sqref="I356"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="11.88671875" customWidth="1"/>
-    <col min="3" max="3" width="13.6640625" customWidth="1"/>
-    <col min="4" max="4" width="26.33203125" customWidth="1"/>
-    <col min="5" max="5" width="18.88671875" customWidth="1"/>
-    <col min="6" max="6" width="19.109375" customWidth="1"/>
+    <col min="2" max="2" width="11.8984375" customWidth="1"/>
+    <col min="3" max="3" width="13.69921875" customWidth="1"/>
+    <col min="4" max="4" width="26.296875" customWidth="1"/>
+    <col min="5" max="5" width="18.8984375" customWidth="1"/>
+    <col min="6" max="6" width="19.09765625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
@@ -6175,7 +6175,7 @@
     </row>
     <row r="239" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A239">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B239" t="s">
         <v>10</v>
@@ -6184,21 +6184,21 @@
         <v>7</v>
       </c>
       <c r="D239" t="s">
-        <v>45</v>
+        <v>9</v>
       </c>
       <c r="E239" t="s">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="F239" t="s">
         <v>7</v>
       </c>
       <c r="G239">
-        <v>3000</v>
+        <v>3500</v>
       </c>
     </row>
     <row r="240" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A240">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B240" t="s">
         <v>10</v>
@@ -6207,7 +6207,7 @@
         <v>7</v>
       </c>
       <c r="D240" t="s">
-        <v>23</v>
+        <v>45</v>
       </c>
       <c r="E240" t="s">
         <v>7</v>
@@ -6221,7 +6221,7 @@
     </row>
     <row r="241" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A241">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="B241" t="s">
         <v>10</v>
@@ -6244,7 +6244,7 @@
     </row>
     <row r="242" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A242">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B242" t="s">
         <v>10</v>
@@ -6253,7 +6253,7 @@
         <v>7</v>
       </c>
       <c r="D242" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E242" t="s">
         <v>7</v>
@@ -6262,12 +6262,12 @@
         <v>7</v>
       </c>
       <c r="G242">
-        <v>3500</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="243" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A243">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="B243" t="s">
         <v>10</v>
@@ -6276,7 +6276,7 @@
         <v>7</v>
       </c>
       <c r="D243" t="s">
-        <v>45</v>
+        <v>24</v>
       </c>
       <c r="E243" t="s">
         <v>7</v>
@@ -6285,12 +6285,12 @@
         <v>7</v>
       </c>
       <c r="G243">
-        <v>3000</v>
+        <v>3500</v>
       </c>
     </row>
     <row r="244" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A244">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B244" t="s">
         <v>10</v>
@@ -6313,7 +6313,7 @@
     </row>
     <row r="245" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A245">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="B245" t="s">
         <v>10</v>
@@ -6322,7 +6322,7 @@
         <v>7</v>
       </c>
       <c r="D245" t="s">
-        <v>23</v>
+        <v>45</v>
       </c>
       <c r="E245" t="s">
         <v>7</v>
@@ -6331,12 +6331,12 @@
         <v>7</v>
       </c>
       <c r="G245">
-        <v>3500</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="246" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A246">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B246" t="s">
         <v>10</v>
@@ -6345,7 +6345,7 @@
         <v>7</v>
       </c>
       <c r="D246" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
       <c r="E246" t="s">
         <v>7</v>
@@ -6354,12 +6354,12 @@
         <v>7</v>
       </c>
       <c r="G246">
-        <v>3000</v>
+        <v>3500</v>
       </c>
     </row>
     <row r="247" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A247">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="B247" t="s">
         <v>10</v>
@@ -6382,16 +6382,16 @@
     </row>
     <row r="248" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A248">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="B248" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C248" t="s">
         <v>7</v>
       </c>
       <c r="D248" t="s">
-        <v>68</v>
+        <v>45</v>
       </c>
       <c r="E248" t="s">
         <v>7</v>
@@ -6400,21 +6400,21 @@
         <v>7</v>
       </c>
       <c r="G248">
-        <v>4500</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="249" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A249">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="B249" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C249" t="s">
         <v>7</v>
       </c>
       <c r="D249" t="s">
-        <v>23</v>
+        <v>68</v>
       </c>
       <c r="E249" t="s">
         <v>7</v>
@@ -6423,12 +6423,12 @@
         <v>7</v>
       </c>
       <c r="G249">
-        <v>3500</v>
+        <v>4500</v>
       </c>
     </row>
     <row r="250" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A250">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="B250" t="s">
         <v>10</v>
@@ -6437,7 +6437,7 @@
         <v>7</v>
       </c>
       <c r="D250" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E250" t="s">
         <v>7</v>
@@ -6451,16 +6451,16 @@
     </row>
     <row r="251" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A251">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="B251" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C251" t="s">
         <v>7</v>
       </c>
       <c r="D251" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="E251" t="s">
         <v>7</v>
@@ -6469,12 +6469,12 @@
         <v>7</v>
       </c>
       <c r="G251">
-        <v>4000</v>
+        <v>3500</v>
       </c>
     </row>
     <row r="252" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A252">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="B252" t="s">
         <v>8</v>
@@ -6483,7 +6483,7 @@
         <v>7</v>
       </c>
       <c r="D252" t="s">
-        <v>46</v>
+        <v>12</v>
       </c>
       <c r="E252" t="s">
         <v>7</v>
@@ -6497,7 +6497,7 @@
     </row>
     <row r="253" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A253">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="B253" t="s">
         <v>8</v>
@@ -6506,21 +6506,21 @@
         <v>7</v>
       </c>
       <c r="D253" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="E253" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="F253" t="s">
         <v>7</v>
       </c>
       <c r="G253">
-        <v>3000</v>
+        <v>4000</v>
       </c>
     </row>
     <row r="254" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A254">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="B254" t="s">
         <v>8</v>
@@ -6529,10 +6529,10 @@
         <v>7</v>
       </c>
       <c r="D254" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="E254" t="s">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="F254" t="s">
         <v>7</v>
@@ -6543,7 +6543,7 @@
     </row>
     <row r="255" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A255">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B255" t="s">
         <v>8</v>
@@ -6552,7 +6552,7 @@
         <v>7</v>
       </c>
       <c r="D255" t="s">
-        <v>54</v>
+        <v>16</v>
       </c>
       <c r="E255" t="s">
         <v>7</v>
@@ -6561,12 +6561,12 @@
         <v>7</v>
       </c>
       <c r="G255">
-        <v>3500</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="256" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A256">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B256" t="s">
         <v>8</v>
@@ -6575,7 +6575,7 @@
         <v>7</v>
       </c>
       <c r="D256" t="s">
-        <v>16</v>
+        <v>54</v>
       </c>
       <c r="E256" t="s">
         <v>7</v>
@@ -6584,12 +6584,12 @@
         <v>7</v>
       </c>
       <c r="G256">
-        <v>2500</v>
+        <v>3500</v>
       </c>
     </row>
     <row r="257" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A257">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B257" t="s">
         <v>8</v>
@@ -6598,7 +6598,7 @@
         <v>7</v>
       </c>
       <c r="D257" t="s">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="E257" t="s">
         <v>7</v>
@@ -6607,12 +6607,12 @@
         <v>7</v>
       </c>
       <c r="G257">
-        <v>4000</v>
+        <v>2500</v>
       </c>
     </row>
     <row r="258" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A258">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="B258" t="s">
         <v>8</v>
@@ -6621,21 +6621,21 @@
         <v>7</v>
       </c>
       <c r="D258" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E258" t="s">
-        <v>69</v>
+        <v>7</v>
       </c>
       <c r="F258" t="s">
         <v>7</v>
       </c>
       <c r="G258">
-        <v>3000</v>
+        <v>4000</v>
       </c>
     </row>
     <row r="259" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A259">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B259" t="s">
         <v>8</v>
@@ -6644,30 +6644,30 @@
         <v>7</v>
       </c>
       <c r="D259" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="E259" t="s">
-        <v>7</v>
+        <v>69</v>
       </c>
       <c r="F259" t="s">
         <v>7</v>
       </c>
       <c r="G259">
-        <v>4500</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="260" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A260">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="B260" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C260" t="s">
         <v>7</v>
       </c>
       <c r="D260" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="E260" t="s">
         <v>7</v>
@@ -6676,21 +6676,21 @@
         <v>7</v>
       </c>
       <c r="G260">
-        <v>3500</v>
+        <v>4500</v>
       </c>
     </row>
     <row r="261" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A261">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B261" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C261" t="s">
         <v>7</v>
       </c>
       <c r="D261" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="E261" t="s">
         <v>7</v>
@@ -6699,12 +6699,12 @@
         <v>7</v>
       </c>
       <c r="G261">
-        <v>4500</v>
+        <v>3500</v>
       </c>
     </row>
     <row r="262" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A262">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B262" t="s">
         <v>8</v>
@@ -6713,7 +6713,7 @@
         <v>7</v>
       </c>
       <c r="D262" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E262" t="s">
         <v>7</v>
@@ -6722,12 +6722,12 @@
         <v>7</v>
       </c>
       <c r="G262">
-        <v>2500</v>
+        <v>4500</v>
       </c>
     </row>
     <row r="263" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A263">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="B263" t="s">
         <v>8</v>
@@ -6736,7 +6736,7 @@
         <v>7</v>
       </c>
       <c r="D263" t="s">
-        <v>38</v>
+        <v>16</v>
       </c>
       <c r="E263" t="s">
         <v>7</v>
@@ -6745,12 +6745,12 @@
         <v>7</v>
       </c>
       <c r="G263">
-        <v>4000</v>
+        <v>2500</v>
       </c>
     </row>
     <row r="264" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A264">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="B264" t="s">
         <v>8</v>
@@ -6759,44 +6759,44 @@
         <v>7</v>
       </c>
       <c r="D264" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="E264" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="F264" t="s">
         <v>7</v>
       </c>
       <c r="G264">
-        <v>3500</v>
+        <v>4000</v>
       </c>
     </row>
     <row r="265" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A265">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B265" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C265" t="s">
         <v>7</v>
       </c>
       <c r="D265" t="s">
-        <v>45</v>
+        <v>27</v>
       </c>
       <c r="E265" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="F265" t="s">
         <v>7</v>
       </c>
       <c r="G265">
-        <v>3000</v>
+        <v>3500</v>
       </c>
     </row>
     <row r="266" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A266">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="B266" t="s">
         <v>10</v>
@@ -6819,16 +6819,16 @@
     </row>
     <row r="267" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A267">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="B267" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C267" t="s">
         <v>7</v>
       </c>
       <c r="D267" t="s">
-        <v>29</v>
+        <v>45</v>
       </c>
       <c r="E267" t="s">
         <v>7</v>
@@ -6837,21 +6837,21 @@
         <v>7</v>
       </c>
       <c r="G267">
-        <v>4000</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="268" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A268">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="B268" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C268" t="s">
         <v>7</v>
       </c>
       <c r="D268" t="s">
-        <v>45</v>
+        <v>29</v>
       </c>
       <c r="E268" t="s">
         <v>7</v>
@@ -6860,21 +6860,21 @@
         <v>7</v>
       </c>
       <c r="G268">
-        <v>3000</v>
+        <v>4000</v>
       </c>
     </row>
     <row r="269" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A269">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B269" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C269" t="s">
         <v>7</v>
       </c>
       <c r="D269" t="s">
-        <v>70</v>
+        <v>45</v>
       </c>
       <c r="E269" t="s">
         <v>7</v>
@@ -6883,12 +6883,12 @@
         <v>7</v>
       </c>
       <c r="G269">
-        <v>3500</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="270" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A270">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="B270" t="s">
         <v>8</v>
@@ -6897,7 +6897,7 @@
         <v>7</v>
       </c>
       <c r="D270" t="s">
-        <v>27</v>
+        <v>70</v>
       </c>
       <c r="E270" t="s">
         <v>7</v>
@@ -6911,7 +6911,7 @@
     </row>
     <row r="271" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A271">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="B271" t="s">
         <v>8</v>
@@ -6929,12 +6929,12 @@
         <v>7</v>
       </c>
       <c r="G271">
-        <v>3000</v>
+        <v>3500</v>
       </c>
     </row>
     <row r="272" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A272">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="B272" t="s">
         <v>8</v>
@@ -6952,12 +6952,12 @@
         <v>7</v>
       </c>
       <c r="G272">
-        <v>4000</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="273" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A273">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="B273" t="s">
         <v>8</v>
@@ -6966,7 +6966,7 @@
         <v>7</v>
       </c>
       <c r="D273" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E273" t="s">
         <v>7</v>
@@ -6975,12 +6975,12 @@
         <v>7</v>
       </c>
       <c r="G273">
-        <v>3500</v>
+        <v>4000</v>
       </c>
     </row>
     <row r="274" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A274">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="B274" t="s">
         <v>8</v>
@@ -6989,7 +6989,7 @@
         <v>7</v>
       </c>
       <c r="D274" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E274" t="s">
         <v>7</v>
@@ -6998,12 +6998,12 @@
         <v>7</v>
       </c>
       <c r="G274">
-        <v>4000</v>
+        <v>3500</v>
       </c>
     </row>
     <row r="275" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A275">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B275" t="s">
         <v>8</v>
@@ -7012,7 +7012,7 @@
         <v>7</v>
       </c>
       <c r="D275" t="s">
-        <v>71</v>
+        <v>27</v>
       </c>
       <c r="E275" t="s">
         <v>7</v>
@@ -7021,12 +7021,12 @@
         <v>7</v>
       </c>
       <c r="G275">
-        <v>4500</v>
+        <v>4000</v>
       </c>
     </row>
     <row r="276" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A276">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="B276" t="s">
         <v>8</v>
@@ -7035,7 +7035,7 @@
         <v>7</v>
       </c>
       <c r="D276" t="s">
-        <v>27</v>
+        <v>71</v>
       </c>
       <c r="E276" t="s">
         <v>7</v>
@@ -7044,12 +7044,12 @@
         <v>7</v>
       </c>
       <c r="G276">
-        <v>3000</v>
+        <v>4500</v>
       </c>
     </row>
     <row r="277" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A277">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="B277" t="s">
         <v>8</v>
@@ -7058,21 +7058,21 @@
         <v>7</v>
       </c>
       <c r="D277" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E277" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="F277" t="s">
         <v>7</v>
       </c>
       <c r="G277">
-        <v>3500</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="278" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A278">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="B278" t="s">
         <v>8</v>
@@ -7081,21 +7081,21 @@
         <v>7</v>
       </c>
       <c r="D278" t="s">
-        <v>72</v>
+        <v>30</v>
       </c>
       <c r="E278" t="s">
-        <v>7</v>
+        <v>33</v>
       </c>
       <c r="F278" t="s">
         <v>7</v>
       </c>
       <c r="G278">
-        <v>4000</v>
+        <v>3500</v>
       </c>
     </row>
     <row r="279" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A279">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="B279" t="s">
         <v>8</v>
@@ -7104,21 +7104,21 @@
         <v>7</v>
       </c>
       <c r="D279" t="s">
-        <v>12</v>
+        <v>72</v>
       </c>
       <c r="E279" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="F279" t="s">
         <v>7</v>
       </c>
       <c r="G279">
-        <v>3500</v>
+        <v>4000</v>
       </c>
     </row>
     <row r="280" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A280">
-        <v>494</v>
+        <v>490</v>
       </c>
       <c r="B280" t="s">
         <v>8</v>
@@ -7127,21 +7127,21 @@
         <v>7</v>
       </c>
       <c r="D280" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="E280" t="s">
-        <v>7</v>
+        <v>33</v>
       </c>
       <c r="F280" t="s">
         <v>7</v>
       </c>
       <c r="G280">
-        <v>4500</v>
+        <v>3500</v>
       </c>
     </row>
     <row r="281" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A281">
-        <v>498</v>
+        <v>494</v>
       </c>
       <c r="B281" t="s">
         <v>8</v>
@@ -7150,7 +7150,7 @@
         <v>7</v>
       </c>
       <c r="D281" t="s">
-        <v>57</v>
+        <v>29</v>
       </c>
       <c r="E281" t="s">
         <v>7</v>
@@ -7159,12 +7159,12 @@
         <v>7</v>
       </c>
       <c r="G281">
-        <v>3500</v>
+        <v>4500</v>
       </c>
     </row>
     <row r="282" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A282">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B282" t="s">
         <v>8</v>
@@ -7173,7 +7173,7 @@
         <v>7</v>
       </c>
       <c r="D282" t="s">
-        <v>29</v>
+        <v>57</v>
       </c>
       <c r="E282" t="s">
         <v>7</v>
@@ -7182,12 +7182,12 @@
         <v>7</v>
       </c>
       <c r="G282">
-        <v>4500</v>
+        <v>3500</v>
       </c>
     </row>
     <row r="283" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A283">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="B283" t="s">
         <v>8</v>
@@ -7196,21 +7196,21 @@
         <v>7</v>
       </c>
       <c r="D283" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E283" t="s">
-        <v>51</v>
+        <v>7</v>
       </c>
       <c r="F283" t="s">
         <v>7</v>
       </c>
       <c r="G283">
-        <v>3500</v>
+        <v>4500</v>
       </c>
     </row>
     <row r="284" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A284">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="B284" t="s">
         <v>8</v>
@@ -7219,21 +7219,21 @@
         <v>7</v>
       </c>
       <c r="D284" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E284" t="s">
-        <v>7</v>
+        <v>51</v>
       </c>
       <c r="F284" t="s">
         <v>7</v>
       </c>
       <c r="G284">
-        <v>2500</v>
+        <v>3500</v>
       </c>
     </row>
     <row r="285" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A285">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="B285" t="s">
         <v>8</v>
@@ -7256,7 +7256,7 @@
     </row>
     <row r="286" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A286">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="B286" t="s">
         <v>8</v>
@@ -7265,7 +7265,7 @@
         <v>7</v>
       </c>
       <c r="D286" t="s">
-        <v>61</v>
+        <v>31</v>
       </c>
       <c r="E286" t="s">
         <v>7</v>
@@ -7274,12 +7274,12 @@
         <v>7</v>
       </c>
       <c r="G286">
-        <v>3000</v>
+        <v>2500</v>
       </c>
     </row>
     <row r="287" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A287">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="B287" t="s">
         <v>8</v>
@@ -7288,7 +7288,7 @@
         <v>7</v>
       </c>
       <c r="D287" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="E287" t="s">
         <v>7</v>
@@ -7297,12 +7297,12 @@
         <v>7</v>
       </c>
       <c r="G287">
-        <v>4000</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="288" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A288">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="B288" t="s">
         <v>8</v>
@@ -7311,21 +7311,21 @@
         <v>7</v>
       </c>
       <c r="D288" t="s">
-        <v>27</v>
+        <v>48</v>
       </c>
       <c r="E288" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="F288" t="s">
         <v>7</v>
       </c>
       <c r="G288">
-        <v>3500</v>
+        <v>4000</v>
       </c>
     </row>
     <row r="289" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A289">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="B289" t="s">
         <v>8</v>
@@ -7337,18 +7337,18 @@
         <v>27</v>
       </c>
       <c r="E289" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="F289" t="s">
         <v>7</v>
       </c>
       <c r="G289">
-        <v>4000</v>
+        <v>3500</v>
       </c>
     </row>
     <row r="290" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A290">
-        <v>516</v>
+        <v>507</v>
       </c>
       <c r="B290" t="s">
         <v>8</v>
@@ -7357,7 +7357,7 @@
         <v>7</v>
       </c>
       <c r="D290" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="E290" t="s">
         <v>7</v>
@@ -7366,12 +7366,12 @@
         <v>7</v>
       </c>
       <c r="G290">
-        <v>3500</v>
+        <v>4000</v>
       </c>
     </row>
     <row r="291" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A291">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="B291" t="s">
         <v>8</v>
@@ -7380,7 +7380,7 @@
         <v>7</v>
       </c>
       <c r="D291" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
       <c r="E291" t="s">
         <v>7</v>
@@ -7389,12 +7389,12 @@
         <v>7</v>
       </c>
       <c r="G291">
-        <v>4500</v>
+        <v>3500</v>
       </c>
     </row>
     <row r="292" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A292">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="B292" t="s">
         <v>8</v>
@@ -7403,7 +7403,7 @@
         <v>7</v>
       </c>
       <c r="D292" t="s">
-        <v>48</v>
+        <v>29</v>
       </c>
       <c r="E292" t="s">
         <v>7</v>
@@ -7412,12 +7412,12 @@
         <v>7</v>
       </c>
       <c r="G292">
-        <v>4000</v>
+        <v>4500</v>
       </c>
     </row>
     <row r="293" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A293">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="B293" t="s">
         <v>8</v>
@@ -7426,7 +7426,7 @@
         <v>7</v>
       </c>
       <c r="D293" t="s">
-        <v>29</v>
+        <v>48</v>
       </c>
       <c r="E293" t="s">
         <v>7</v>
@@ -7435,12 +7435,12 @@
         <v>7</v>
       </c>
       <c r="G293">
-        <v>4500</v>
+        <v>4000</v>
       </c>
     </row>
     <row r="294" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A294">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="B294" t="s">
         <v>8</v>
@@ -7449,33 +7449,33 @@
         <v>7</v>
       </c>
       <c r="D294" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E294" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="F294" t="s">
         <v>7</v>
       </c>
       <c r="G294">
-        <v>3000</v>
+        <v>4500</v>
       </c>
     </row>
     <row r="295" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A295">
-        <v>526</v>
+        <v>522</v>
       </c>
       <c r="B295" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C295" t="s">
         <v>7</v>
       </c>
       <c r="D295" t="s">
-        <v>45</v>
+        <v>27</v>
       </c>
       <c r="E295" t="s">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="F295" t="s">
         <v>7</v>
@@ -7486,16 +7486,16 @@
     </row>
     <row r="296" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A296">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="B296" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C296" t="s">
         <v>7</v>
       </c>
       <c r="D296" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="E296" t="s">
         <v>7</v>
@@ -7504,12 +7504,12 @@
         <v>7</v>
       </c>
       <c r="G296">
-        <v>3500</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="297" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A297">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="B297" t="s">
         <v>8</v>
@@ -7518,7 +7518,7 @@
         <v>7</v>
       </c>
       <c r="D297" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="E297" t="s">
         <v>7</v>
@@ -7527,12 +7527,12 @@
         <v>7</v>
       </c>
       <c r="G297">
-        <v>4500</v>
+        <v>3500</v>
       </c>
     </row>
     <row r="298" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A298">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="B298" t="s">
         <v>8</v>
@@ -7541,7 +7541,7 @@
         <v>7</v>
       </c>
       <c r="D298" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="E298" t="s">
         <v>7</v>
@@ -7555,7 +7555,7 @@
     </row>
     <row r="299" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A299">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="B299" t="s">
         <v>8</v>
@@ -7564,21 +7564,21 @@
         <v>7</v>
       </c>
       <c r="D299" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="E299" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="F299" t="s">
         <v>7</v>
       </c>
       <c r="G299">
-        <v>3500</v>
+        <v>4500</v>
       </c>
     </row>
     <row r="300" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A300">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="B300" t="s">
         <v>8</v>
@@ -7587,53 +7587,53 @@
         <v>7</v>
       </c>
       <c r="D300" t="s">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="E300" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="F300" t="s">
         <v>7</v>
       </c>
       <c r="G300">
-        <v>2500</v>
+        <v>3500</v>
       </c>
     </row>
     <row r="301" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A301">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="B301" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C301" t="s">
         <v>7</v>
       </c>
       <c r="D301" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="E301" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="F301" t="s">
         <v>7</v>
       </c>
       <c r="G301">
-        <v>3500</v>
+        <v>2500</v>
       </c>
     </row>
     <row r="302" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A302">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="B302" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C302" t="s">
         <v>7</v>
       </c>
       <c r="D302" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="E302" t="s">
         <v>7</v>
@@ -7647,7 +7647,7 @@
     </row>
     <row r="303" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A303">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="B303" t="s">
         <v>8</v>
@@ -7656,7 +7656,7 @@
         <v>7</v>
       </c>
       <c r="D303" t="s">
-        <v>29</v>
+        <v>6</v>
       </c>
       <c r="E303" t="s">
         <v>7</v>
@@ -7670,7 +7670,7 @@
     </row>
     <row r="304" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A304">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="B304" t="s">
         <v>8</v>
@@ -7679,7 +7679,7 @@
         <v>7</v>
       </c>
       <c r="D304" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="E304" t="s">
         <v>7</v>
@@ -7688,12 +7688,12 @@
         <v>7</v>
       </c>
       <c r="G304">
-        <v>4000</v>
+        <v>3500</v>
       </c>
     </row>
     <row r="305" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A305">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="B305" t="s">
         <v>8</v>
@@ -7702,7 +7702,7 @@
         <v>7</v>
       </c>
       <c r="D305" t="s">
-        <v>36</v>
+        <v>12</v>
       </c>
       <c r="E305" t="s">
         <v>7</v>
@@ -7711,12 +7711,12 @@
         <v>7</v>
       </c>
       <c r="G305">
-        <v>3000</v>
+        <v>4000</v>
       </c>
     </row>
     <row r="306" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A306">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="B306" t="s">
         <v>8</v>
@@ -7725,7 +7725,7 @@
         <v>7</v>
       </c>
       <c r="D306" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="E306" t="s">
         <v>7</v>
@@ -7739,7 +7739,7 @@
     </row>
     <row r="307" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A307">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="B307" t="s">
         <v>8</v>
@@ -7748,7 +7748,7 @@
         <v>7</v>
       </c>
       <c r="D307" t="s">
-        <v>73</v>
+        <v>27</v>
       </c>
       <c r="E307" t="s">
         <v>7</v>
@@ -7757,21 +7757,21 @@
         <v>7</v>
       </c>
       <c r="G307">
-        <v>3500</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="308" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A308">
-        <v>543</v>
+        <v>540</v>
       </c>
       <c r="B308" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C308" t="s">
         <v>7</v>
       </c>
       <c r="D308" t="s">
-        <v>9</v>
+        <v>73</v>
       </c>
       <c r="E308" t="s">
         <v>7</v>
@@ -7785,30 +7785,30 @@
     </row>
     <row r="309" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A309">
-        <v>546</v>
+        <v>543</v>
       </c>
       <c r="B309" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C309" t="s">
         <v>7</v>
       </c>
       <c r="D309" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E309" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="F309" t="s">
         <v>7</v>
       </c>
       <c r="G309">
-        <v>2500</v>
+        <v>3500</v>
       </c>
     </row>
     <row r="310" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A310">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="B310" t="s">
         <v>8</v>
@@ -7817,10 +7817,10 @@
         <v>7</v>
       </c>
       <c r="D310" t="s">
-        <v>40</v>
+        <v>14</v>
       </c>
       <c r="E310" t="s">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="F310" t="s">
         <v>7</v>
@@ -7831,7 +7831,7 @@
     </row>
     <row r="311" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A311">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="B311" t="s">
         <v>8</v>
@@ -7840,7 +7840,7 @@
         <v>7</v>
       </c>
       <c r="D311" t="s">
-        <v>74</v>
+        <v>40</v>
       </c>
       <c r="E311" t="s">
         <v>7</v>
@@ -7849,21 +7849,21 @@
         <v>7</v>
       </c>
       <c r="G311">
-        <v>3500</v>
+        <v>2500</v>
       </c>
     </row>
     <row r="312" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A312">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="B312" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C312" t="s">
         <v>7</v>
       </c>
       <c r="D312" t="s">
-        <v>45</v>
+        <v>74</v>
       </c>
       <c r="E312" t="s">
         <v>7</v>
@@ -7872,21 +7872,21 @@
         <v>7</v>
       </c>
       <c r="G312">
-        <v>3000</v>
+        <v>3500</v>
       </c>
     </row>
     <row r="313" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A313">
-        <v>552</v>
+        <v>549</v>
       </c>
       <c r="B313" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C313" t="s">
         <v>7</v>
       </c>
       <c r="D313" t="s">
-        <v>27</v>
+        <v>45</v>
       </c>
       <c r="E313" t="s">
         <v>7</v>
@@ -7895,21 +7895,21 @@
         <v>7</v>
       </c>
       <c r="G313">
-        <v>3500</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="314" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A314">
-        <v>555</v>
+        <v>552</v>
       </c>
       <c r="B314" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C314" t="s">
         <v>7</v>
       </c>
       <c r="D314" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="E314" t="s">
         <v>7</v>
@@ -7923,16 +7923,16 @@
     </row>
     <row r="315" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A315">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="B315" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C315" t="s">
         <v>7</v>
       </c>
       <c r="D315" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="E315" t="s">
         <v>7</v>
@@ -7941,21 +7941,21 @@
         <v>7</v>
       </c>
       <c r="G315">
-        <v>4500</v>
+        <v>3500</v>
       </c>
     </row>
     <row r="316" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A316">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="B316" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C316" t="s">
         <v>7</v>
       </c>
       <c r="D316" t="s">
-        <v>75</v>
+        <v>29</v>
       </c>
       <c r="E316" t="s">
         <v>7</v>
@@ -7964,24 +7964,24 @@
         <v>7</v>
       </c>
       <c r="G316">
-        <v>3000</v>
+        <v>4500</v>
       </c>
     </row>
     <row r="317" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A317">
-        <v>562</v>
+        <v>558</v>
       </c>
       <c r="B317" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C317" t="s">
         <v>7</v>
       </c>
       <c r="D317" t="s">
-        <v>27</v>
+        <v>75</v>
       </c>
       <c r="E317" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="F317" t="s">
         <v>7</v>
@@ -7992,7 +7992,7 @@
     </row>
     <row r="318" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A318">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="B318" t="s">
         <v>8</v>
@@ -8001,7 +8001,7 @@
         <v>7</v>
       </c>
       <c r="D318" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="E318" t="s">
         <v>22</v>
@@ -8010,35 +8010,35 @@
         <v>7</v>
       </c>
       <c r="G318">
-        <v>2500</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="319" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A319">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="B319" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C319" t="s">
         <v>7</v>
       </c>
       <c r="D319" t="s">
-        <v>45</v>
+        <v>16</v>
       </c>
       <c r="E319" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="F319" t="s">
         <v>7</v>
       </c>
       <c r="G319">
-        <v>3000</v>
+        <v>2500</v>
       </c>
     </row>
     <row r="320" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A320">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="B320" t="s">
         <v>10</v>
@@ -8047,21 +8047,21 @@
         <v>7</v>
       </c>
       <c r="D320" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="E320" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="F320" t="s">
         <v>7</v>
       </c>
       <c r="G320">
-        <v>2500</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="321" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A321">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="B321" t="s">
         <v>10</v>
@@ -8070,67 +8070,67 @@
         <v>7</v>
       </c>
       <c r="D321" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="E321" t="s">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="F321" t="s">
         <v>7</v>
       </c>
       <c r="G321">
-        <v>3000</v>
+        <v>2500</v>
       </c>
     </row>
     <row r="322" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A322">
-        <v>571</v>
+        <v>566</v>
       </c>
       <c r="B322" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C322" t="s">
         <v>7</v>
       </c>
       <c r="D322" t="s">
-        <v>27</v>
+        <v>45</v>
       </c>
       <c r="E322" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="F322" t="s">
         <v>7</v>
       </c>
       <c r="G322">
-        <v>3500</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="323" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A323">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="B323" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C323" t="s">
         <v>7</v>
       </c>
       <c r="D323" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="E323" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="F323" t="s">
         <v>7</v>
       </c>
       <c r="G323">
-        <v>3000</v>
+        <v>3500</v>
       </c>
     </row>
     <row r="324" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A324">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="B324" t="s">
         <v>10</v>
@@ -8139,7 +8139,7 @@
         <v>7</v>
       </c>
       <c r="D324" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="E324" t="s">
         <v>7</v>
@@ -8148,21 +8148,21 @@
         <v>7</v>
       </c>
       <c r="G324">
-        <v>3500</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="325" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A325">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="B325" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C325" t="s">
         <v>7</v>
       </c>
       <c r="D325" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="E325" t="s">
         <v>7</v>
@@ -8171,12 +8171,12 @@
         <v>7</v>
       </c>
       <c r="G325">
-        <v>4000</v>
+        <v>3500</v>
       </c>
     </row>
     <row r="326" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A326">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="B326" t="s">
         <v>8</v>
@@ -8185,7 +8185,7 @@
         <v>7</v>
       </c>
       <c r="D326" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E326" t="s">
         <v>7</v>
@@ -8193,13 +8193,13 @@
       <c r="F326" t="s">
         <v>7</v>
       </c>
-      <c r="G326" t="s">
-        <v>7</v>
+      <c r="G326">
+        <v>4000</v>
       </c>
     </row>
     <row r="327" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A327">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B327" t="s">
         <v>8</v>
@@ -8208,21 +8208,21 @@
         <v>7</v>
       </c>
       <c r="D327" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="E327" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="F327" t="s">
         <v>7</v>
       </c>
-      <c r="G327">
-        <v>3500</v>
+      <c r="G327" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="328" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A328">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="B328" t="s">
         <v>8</v>
@@ -8231,30 +8231,30 @@
         <v>7</v>
       </c>
       <c r="D328" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="E328" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="F328" t="s">
         <v>7</v>
       </c>
       <c r="G328">
-        <v>2500</v>
+        <v>3500</v>
       </c>
     </row>
     <row r="329" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A329">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="B329" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C329" t="s">
         <v>7</v>
       </c>
       <c r="D329" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="E329" t="s">
         <v>7</v>
@@ -8263,24 +8263,24 @@
         <v>7</v>
       </c>
       <c r="G329">
-        <v>3500</v>
+        <v>2500</v>
       </c>
     </row>
     <row r="330" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A330">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="B330" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C330" t="s">
         <v>7</v>
       </c>
       <c r="D330" t="s">
-        <v>30</v>
+        <v>9</v>
       </c>
       <c r="E330" t="s">
-        <v>76</v>
+        <v>7</v>
       </c>
       <c r="F330" t="s">
         <v>7</v>
@@ -8291,7 +8291,7 @@
     </row>
     <row r="331" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A331">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="B331" t="s">
         <v>8</v>
@@ -8303,7 +8303,7 @@
         <v>30</v>
       </c>
       <c r="E331" t="s">
-        <v>33</v>
+        <v>76</v>
       </c>
       <c r="F331" t="s">
         <v>7</v>
@@ -8314,7 +8314,7 @@
     </row>
     <row r="332" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A332">
-        <v>584</v>
+        <v>581</v>
       </c>
       <c r="B332" t="s">
         <v>8</v>
@@ -8326,7 +8326,7 @@
         <v>30</v>
       </c>
       <c r="E332" t="s">
-        <v>7</v>
+        <v>33</v>
       </c>
       <c r="F332" t="s">
         <v>7</v>
@@ -8337,7 +8337,7 @@
     </row>
     <row r="333" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A333">
-        <v>587</v>
+        <v>584</v>
       </c>
       <c r="B333" t="s">
         <v>8</v>
@@ -8346,21 +8346,21 @@
         <v>7</v>
       </c>
       <c r="D333" t="s">
-        <v>77</v>
+        <v>30</v>
       </c>
       <c r="E333" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="F333" t="s">
         <v>7</v>
       </c>
-      <c r="G333" t="s">
-        <v>7</v>
+      <c r="G333">
+        <v>3500</v>
       </c>
     </row>
     <row r="334" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A334">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="B334" t="s">
         <v>8</v>
@@ -8369,10 +8369,10 @@
         <v>7</v>
       </c>
       <c r="D334" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E334" t="s">
-        <v>79</v>
+        <v>15</v>
       </c>
       <c r="F334" t="s">
         <v>7</v>
@@ -8383,7 +8383,7 @@
     </row>
     <row r="335" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A335">
-        <v>591</v>
+        <v>588</v>
       </c>
       <c r="B335" t="s">
         <v>8</v>
@@ -8392,21 +8392,21 @@
         <v>7</v>
       </c>
       <c r="D335" t="s">
-        <v>31</v>
+        <v>78</v>
       </c>
       <c r="E335" t="s">
-        <v>7</v>
+        <v>79</v>
       </c>
       <c r="F335" t="s">
         <v>7</v>
       </c>
-      <c r="G335">
-        <v>2500</v>
+      <c r="G335" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="336" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A336">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="B336" t="s">
         <v>8</v>
@@ -8415,18 +8415,21 @@
         <v>7</v>
       </c>
       <c r="D336" t="s">
-        <v>80</v>
+        <v>31</v>
+      </c>
+      <c r="E336" t="s">
+        <v>7</v>
       </c>
       <c r="F336" t="s">
         <v>7</v>
       </c>
       <c r="G336">
-        <v>4000</v>
+        <v>2500</v>
       </c>
     </row>
     <row r="337" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A337">
-        <v>595</v>
+        <v>592</v>
       </c>
       <c r="B337" t="s">
         <v>8</v>
@@ -8435,21 +8438,18 @@
         <v>7</v>
       </c>
       <c r="D337" t="s">
-        <v>59</v>
-      </c>
-      <c r="E337" t="s">
-        <v>7</v>
+        <v>80</v>
       </c>
       <c r="F337" t="s">
         <v>7</v>
       </c>
       <c r="G337">
-        <v>3500</v>
+        <v>4000</v>
       </c>
     </row>
     <row r="338" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A338">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="B338" t="s">
         <v>8</v>
@@ -8458,18 +8458,21 @@
         <v>7</v>
       </c>
       <c r="D338" t="s">
-        <v>81</v>
+        <v>59</v>
+      </c>
+      <c r="E338" t="s">
+        <v>7</v>
       </c>
       <c r="F338" t="s">
         <v>7</v>
       </c>
-      <c r="G338" t="s">
-        <v>7</v>
+      <c r="G338">
+        <v>3500</v>
       </c>
     </row>
     <row r="339" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A339">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="B339" t="s">
         <v>8</v>
@@ -8478,21 +8481,18 @@
         <v>7</v>
       </c>
       <c r="D339" t="s">
-        <v>82</v>
-      </c>
-      <c r="E339" t="s">
-        <v>28</v>
+        <v>81</v>
       </c>
       <c r="F339" t="s">
         <v>7</v>
       </c>
-      <c r="G339">
-        <v>3000</v>
+      <c r="G339" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="340" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A340">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="B340" t="s">
         <v>8</v>
@@ -8501,21 +8501,21 @@
         <v>7</v>
       </c>
       <c r="D340" t="s">
-        <v>29</v>
+        <v>82</v>
       </c>
       <c r="E340" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="F340" t="s">
         <v>7</v>
       </c>
       <c r="G340">
-        <v>3500</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="341" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A341">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="B341" t="s">
         <v>8</v>
@@ -8524,18 +8524,21 @@
         <v>7</v>
       </c>
       <c r="D341" t="s">
-        <v>83</v>
+        <v>29</v>
+      </c>
+      <c r="E341" t="s">
+        <v>22</v>
       </c>
       <c r="F341" t="s">
         <v>7</v>
       </c>
-      <c r="G341" t="s">
-        <v>7</v>
+      <c r="G341">
+        <v>3500</v>
       </c>
     </row>
     <row r="342" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A342">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="B342" t="s">
         <v>8</v>
@@ -8544,21 +8547,18 @@
         <v>7</v>
       </c>
       <c r="D342" t="s">
-        <v>40</v>
-      </c>
-      <c r="E342" t="s">
-        <v>7</v>
+        <v>83</v>
       </c>
       <c r="F342" t="s">
         <v>7</v>
       </c>
-      <c r="G342">
-        <v>2500</v>
+      <c r="G342" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="343" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A343">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="B343" t="s">
         <v>8</v>
@@ -8567,7 +8567,7 @@
         <v>7</v>
       </c>
       <c r="D343" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="E343" t="s">
         <v>7</v>
@@ -8576,12 +8576,12 @@
         <v>7</v>
       </c>
       <c r="G343">
-        <v>3500</v>
+        <v>2500</v>
       </c>
     </row>
     <row r="344" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A344">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="B344" t="s">
         <v>8</v>
@@ -8590,21 +8590,21 @@
         <v>7</v>
       </c>
       <c r="D344" t="s">
-        <v>84</v>
+        <v>30</v>
       </c>
       <c r="E344" t="s">
-        <v>85</v>
+        <v>7</v>
       </c>
       <c r="F344" t="s">
         <v>7</v>
       </c>
-      <c r="G344" t="s">
-        <v>7</v>
+      <c r="G344">
+        <v>3500</v>
       </c>
     </row>
     <row r="345" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A345">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="B345" t="s">
         <v>8</v>
@@ -8613,7 +8613,7 @@
         <v>7</v>
       </c>
       <c r="D345" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E345" t="s">
         <v>85</v>
@@ -8627,7 +8627,7 @@
     </row>
     <row r="346" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A346">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="B346" t="s">
         <v>8</v>
@@ -8636,10 +8636,10 @@
         <v>7</v>
       </c>
       <c r="D346" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E346" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="F346" t="s">
         <v>7</v>
@@ -8650,39 +8650,39 @@
     </row>
     <row r="347" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A347">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="B347" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C347" t="s">
         <v>7</v>
       </c>
       <c r="D347" t="s">
-        <v>50</v>
+        <v>87</v>
       </c>
       <c r="E347" t="s">
-        <v>7</v>
+        <v>88</v>
       </c>
       <c r="F347" t="s">
         <v>7</v>
       </c>
-      <c r="G347">
-        <v>4000</v>
+      <c r="G347" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="348" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A348">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="B348" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C348" t="s">
         <v>7</v>
       </c>
       <c r="D348" t="s">
-        <v>29</v>
+        <v>50</v>
       </c>
       <c r="E348" t="s">
         <v>7</v>
@@ -8696,7 +8696,7 @@
     </row>
     <row r="349" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A349">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="B349" t="s">
         <v>8</v>
@@ -8705,21 +8705,21 @@
         <v>7</v>
       </c>
       <c r="D349" t="s">
-        <v>89</v>
+        <v>29</v>
       </c>
       <c r="E349" t="s">
-        <v>85</v>
+        <v>7</v>
       </c>
       <c r="F349" t="s">
         <v>7</v>
       </c>
-      <c r="G349" t="s">
-        <v>7</v>
+      <c r="G349">
+        <v>4000</v>
       </c>
     </row>
     <row r="350" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A350">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="B350" t="s">
         <v>8</v>
@@ -8728,21 +8728,21 @@
         <v>7</v>
       </c>
       <c r="D350" t="s">
-        <v>31</v>
+        <v>89</v>
       </c>
       <c r="E350" t="s">
-        <v>7</v>
+        <v>85</v>
       </c>
       <c r="F350" t="s">
         <v>7</v>
       </c>
-      <c r="G350">
-        <v>2500</v>
+      <c r="G350" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="351" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A351">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="B351" t="s">
         <v>8</v>
@@ -8751,67 +8751,67 @@
         <v>7</v>
       </c>
       <c r="D351" t="s">
-        <v>90</v>
+        <v>31</v>
       </c>
       <c r="E351" t="s">
-        <v>85</v>
+        <v>7</v>
       </c>
       <c r="F351" t="s">
         <v>7</v>
       </c>
-      <c r="G351" t="s">
-        <v>7</v>
+      <c r="G351">
+        <v>2500</v>
       </c>
     </row>
     <row r="352" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A352">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="B352" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C352" t="s">
         <v>7</v>
       </c>
       <c r="D352" t="s">
-        <v>45</v>
+        <v>90</v>
       </c>
       <c r="E352" t="s">
-        <v>7</v>
+        <v>85</v>
       </c>
       <c r="F352" t="s">
         <v>7</v>
       </c>
-      <c r="G352">
-        <v>3000</v>
+      <c r="G352" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="353" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A353">
-        <v>616</v>
+        <v>610</v>
       </c>
       <c r="B353" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C353" t="s">
         <v>7</v>
       </c>
       <c r="D353" t="s">
-        <v>91</v>
+        <v>45</v>
       </c>
       <c r="E353" t="s">
-        <v>88</v>
+        <v>7</v>
       </c>
       <c r="F353" t="s">
         <v>7</v>
       </c>
-      <c r="G353" t="s">
-        <v>7</v>
+      <c r="G353">
+        <v>3000</v>
       </c>
     </row>
     <row r="354" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A354">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="B354" t="s">
         <v>8</v>
@@ -8823,7 +8823,7 @@
         <v>91</v>
       </c>
       <c r="E354" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="F354" t="s">
         <v>7</v>
@@ -8834,7 +8834,7 @@
     </row>
     <row r="355" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A355">
-        <v>624</v>
+        <v>618</v>
       </c>
       <c r="B355" t="s">
         <v>8</v>
@@ -8843,10 +8843,10 @@
         <v>7</v>
       </c>
       <c r="D355" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="E355" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="F355" t="s">
         <v>7</v>
@@ -8857,7 +8857,7 @@
     </row>
     <row r="356" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A356">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="B356" t="s">
         <v>8</v>
@@ -8866,38 +8866,61 @@
         <v>7</v>
       </c>
       <c r="D356" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="E356" t="s">
-        <v>28</v>
+        <v>88</v>
       </c>
       <c r="F356" t="s">
         <v>7</v>
       </c>
-      <c r="G356">
-        <v>3000</v>
+      <c r="G356" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="357" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A357">
+        <v>625</v>
+      </c>
+      <c r="B357" t="s">
+        <v>8</v>
+      </c>
+      <c r="C357" t="s">
+        <v>7</v>
+      </c>
+      <c r="D357" t="s">
+        <v>92</v>
+      </c>
+      <c r="E357" t="s">
+        <v>28</v>
+      </c>
+      <c r="F357" t="s">
+        <v>7</v>
+      </c>
+      <c r="G357">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="358" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A358">
         <v>630</v>
       </c>
-      <c r="B357" t="s">
-        <v>8</v>
-      </c>
-      <c r="C357" t="s">
-        <v>7</v>
-      </c>
-      <c r="D357" t="s">
+      <c r="B358" t="s">
+        <v>8</v>
+      </c>
+      <c r="C358" t="s">
+        <v>7</v>
+      </c>
+      <c r="D358" t="s">
         <v>93</v>
       </c>
-      <c r="E357" t="s">
+      <c r="E358" t="s">
         <v>94</v>
       </c>
-      <c r="F357" t="s">
-        <v>7</v>
-      </c>
-      <c r="G357" t="s">
+      <c r="F358" t="s">
+        <v>7</v>
+      </c>
+      <c r="G358" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>